<commit_message>
Update for utils to support higher dim datasets, cleaning, restructuring
</commit_message>
<xml_diff>
--- a/Results/Notebook 2 Example 1/Scores/average_scores.xlsx
+++ b/Results/Notebook 2 Example 1/Scores/average_scores.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -459,12 +459,12 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>0.017±0.004</t>
+          <t>0.016±0.003</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.197±0.023</t>
+          <t>0.195±0.014</t>
         </is>
       </c>
     </row>
@@ -476,12 +476,12 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>0.067±0.010</t>
+          <t>0.071±0.008</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.233±0.042</t>
+          <t>0.201±0.048</t>
         </is>
       </c>
     </row>
@@ -493,12 +493,12 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>0.780±0.148</t>
+          <t>0.784±0.124</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.282±0.126</t>
+          <t>0.328±0.155</t>
         </is>
       </c>
     </row>
@@ -510,12 +510,12 @@
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>0.978±0.015</t>
+          <t>0.981±0.014</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.339±0.033</t>
+          <t>0.408±0.033</t>
         </is>
       </c>
     </row>
@@ -527,12 +527,12 @@
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>0.952±0.048</t>
+          <t>0.939±0.048</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.657±0.115</t>
+          <t>0.702±0.104</t>
         </is>
       </c>
     </row>
@@ -544,12 +544,12 @@
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>0.845±0.147</t>
+          <t>0.846±0.125</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.172±0.095</t>
+          <t>0.217±0.116</t>
         </is>
       </c>
     </row>
@@ -561,12 +561,12 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>0.004±0.002</t>
+          <t>0.006±0.003</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.211±0.027</t>
+          <t>0.192±0.016</t>
         </is>
       </c>
     </row>

</xml_diff>